<commit_message>
SLS Implicit Unit Test Updated Version 3.0
</commit_message>
<xml_diff>
--- a/UnitTests/TuningCorrector/test_11 Manual SLS Implicit/8/180613MadixKo_Test_11_TC_1butanal_SLS_Implicit.xlsx
+++ b/UnitTests/TuningCorrector/test_11 Manual SLS Implicit/8/180613MadixKo_Test_11_TC_1butanal_SLS_Implicit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Data Analysis/220310_Implicit_SLS_Unit_Test_11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanel\OneDrive\2021LaneLeeCCIFall2021\Data Analysis\220316_Implicit_SLS_Unit_Test_11_TEMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{8FAFFF76-7F1E-4F57-AA30-C47387B52DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB856F48-777C-449D-BA5E-FFA25A31C13F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D17117-AF16-466E-8281-DF82B4A499BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31455" yWindow="1230" windowWidth="20355" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="7890" windowWidth="30810" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5988,8 +5988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6051,12 +6051,11 @@
         <v>20</v>
       </c>
       <c r="W3" s="14">
-        <f>(6*5)+10+8</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="X3" s="5">
         <f t="shared" ref="X3:X8" si="0">(0.6*(W3/14))+0.4</f>
-        <v>2.4571428571428569</v>
+        <v>2.1142857142857143</v>
       </c>
       <c r="Y3" t="s">
         <v>2</v>
@@ -11372,39 +11371,39 @@
       </c>
       <c r="E55" s="16">
         <f t="shared" si="13"/>
-        <v>3151.2852330263022</v>
+        <v>3662.30446000354</v>
       </c>
       <c r="F55" s="16">
         <f t="shared" si="13"/>
-        <v>1056.724250807333</v>
+        <v>1228.0849401274409</v>
       </c>
       <c r="G55" s="16">
         <f t="shared" si="13"/>
-        <v>199.1648600488513</v>
+        <v>231.4618643810974</v>
       </c>
       <c r="H55" s="16">
         <f t="shared" si="13"/>
-        <v>59.270391093203813</v>
+        <v>68.881805865074682</v>
       </c>
       <c r="I55" s="16">
         <f t="shared" si="13"/>
-        <v>1605.9973661914075</v>
+        <v>1866.4293715197439</v>
       </c>
       <c r="J55" s="16">
         <f t="shared" si="13"/>
-        <v>1073.5874634541196</v>
+        <v>1247.6827277980308</v>
       </c>
       <c r="K55" s="16">
         <f t="shared" si="13"/>
-        <v>215.12402594160199</v>
+        <v>250.0090031213212</v>
       </c>
       <c r="L55" s="16">
         <f t="shared" si="13"/>
-        <v>1615.1290833863882</v>
+        <v>1877.041907719316</v>
       </c>
       <c r="M55" s="16">
         <f t="shared" si="13"/>
-        <v>3230.9385752309449</v>
+        <v>3754.8745604035303</v>
       </c>
       <c r="N55" s="16" t="e">
         <f t="shared" si="13"/>
@@ -11424,27 +11423,27 @@
       </c>
       <c r="R55" s="16">
         <f t="shared" si="13"/>
-        <v>50.37580452415618</v>
+        <v>58.544853906451777</v>
       </c>
       <c r="S55" s="16">
         <f t="shared" si="13"/>
-        <v>5.3622162051968694</v>
+        <v>6.2317647790125772</v>
       </c>
       <c r="T55" s="16">
         <f t="shared" si="13"/>
-        <v>21.066133832619478</v>
+        <v>24.482263643314525</v>
       </c>
       <c r="U55" s="16">
         <f t="shared" si="13"/>
-        <v>5.7912897085895647</v>
+        <v>6.7304177694419254</v>
       </c>
       <c r="V55" s="16">
         <f t="shared" si="13"/>
-        <v>257.83965139670778</v>
+        <v>299.65148675833603</v>
       </c>
       <c r="W55" s="16">
         <f t="shared" si="13"/>
-        <v>109.55247950881126</v>
+        <v>127.31774645618603</v>
       </c>
       <c r="X55" s="16" t="e">
         <f t="shared" si="13"/>
@@ -11460,47 +11459,47 @@
       </c>
       <c r="AA55" s="16">
         <f t="shared" si="13"/>
-        <v>969.18970406672156</v>
+        <v>1126.3556020234873</v>
       </c>
       <c r="AB55" s="16">
         <f t="shared" si="13"/>
-        <v>106.33723888496476</v>
+        <v>123.58111546090498</v>
       </c>
       <c r="AC55" s="16">
         <f t="shared" si="13"/>
-        <v>61.596736278857463</v>
+        <v>71.585396215969496</v>
       </c>
       <c r="AD55" s="16">
         <f t="shared" si="13"/>
-        <v>12.087936672079417</v>
+        <v>14.048142618903105</v>
       </c>
       <c r="AE55" s="16">
         <f t="shared" si="13"/>
-        <v>91.835838147740034</v>
+        <v>106.72813622575191</v>
       </c>
       <c r="AF55" s="16">
         <f t="shared" si="13"/>
-        <v>4.4832468043337377</v>
+        <v>5.2102597996310998</v>
       </c>
       <c r="AG55" s="16">
         <f t="shared" si="13"/>
-        <v>22.447046907842907</v>
+        <v>26.087108568574184</v>
       </c>
       <c r="AH55" s="16">
         <f t="shared" si="13"/>
-        <v>3.3452434063172802</v>
+        <v>3.8877153100444062</v>
       </c>
       <c r="AI55" s="16">
         <f t="shared" si="13"/>
-        <v>2.5897551963251595</v>
+        <v>3.0097154984319414</v>
       </c>
       <c r="AJ55" s="16">
         <f t="shared" si="13"/>
-        <v>72.769404559096998</v>
+        <v>84.569848541653258</v>
       </c>
       <c r="AK55" s="16">
         <f t="shared" si="13"/>
-        <v>626.02566628895602</v>
+        <v>727.54334190338125</v>
       </c>
       <c r="AL55" s="16" t="e">
         <f t="shared" si="13"/>
@@ -11508,47 +11507,47 @@
       </c>
       <c r="AM55" s="16">
         <f t="shared" si="13"/>
-        <v>2418.0469500117702</v>
+        <v>2810.1626716352998</v>
       </c>
       <c r="AN55" s="16">
         <f t="shared" si="13"/>
-        <v>474.99824648096416</v>
+        <v>552.02498915355284</v>
       </c>
       <c r="AO55" s="16">
         <f t="shared" si="13"/>
-        <v>194.33524470171855</v>
+        <v>225.84906816686208</v>
       </c>
       <c r="AP55" s="16">
         <f t="shared" si="13"/>
-        <v>286.15179577912102</v>
+        <v>332.55478968924865</v>
       </c>
       <c r="AQ55" s="16">
         <f t="shared" si="13"/>
-        <v>1123.3160632791046</v>
+        <v>1305.4754248919321</v>
       </c>
       <c r="AR55" s="16">
         <f t="shared" si="13"/>
-        <v>88.173490639594377</v>
+        <v>102.47189452709614</v>
       </c>
       <c r="AS55" s="16">
         <f t="shared" si="13"/>
-        <v>94.016756687737541</v>
+        <v>109.26271723169496</v>
       </c>
       <c r="AT55" s="16">
         <f t="shared" si="13"/>
-        <v>70.694231429965285</v>
+        <v>82.158160851040734</v>
       </c>
       <c r="AU55" s="16">
         <f t="shared" si="13"/>
-        <v>519.9268141914946</v>
+        <v>604.23927054687204</v>
       </c>
       <c r="AV55" s="16">
         <f t="shared" si="13"/>
-        <v>7.8972382443258144</v>
+        <v>9.1778714731354043</v>
       </c>
       <c r="AW55" s="16">
         <f t="shared" si="13"/>
-        <v>181.72199324943389</v>
+        <v>211.1904245871799</v>
       </c>
       <c r="AX55" s="16" t="e">
         <f t="shared" si="13"/>
@@ -11584,7 +11583,7 @@
       </c>
       <c r="BF55" s="16">
         <f t="shared" si="13"/>
-        <v>1472.2734450584635</v>
+        <v>1711.0204902030789</v>
       </c>
     </row>
     <row r="56" spans="2:58" x14ac:dyDescent="0.25">
@@ -13281,7 +13280,7 @@
         <v>39</v>
       </c>
       <c r="D68" s="23">
-        <v>12.087936672079417</v>
+        <v>14.048142618903105</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>20</v>
@@ -13293,7 +13292,7 @@
       </c>
       <c r="K68" s="22">
         <f t="shared" ref="K68:K75" si="23">ROUND(D68,1)</f>
-        <v>12.1</v>
+        <v>14</v>
       </c>
       <c r="R68" s="9" t="s">
         <v>22</v>

</xml_diff>